<commit_message>
fixing author calc of total churn logic in authors_contrib function
</commit_message>
<xml_diff>
--- a/database_tables_visualizer.xlsx
+++ b/database_tables_visualizer.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -1521,7 +1521,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1549,13 +1549,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
       </c>
       <c r="D2">
-        <v>0.8666666666666667</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1566,16 +1566,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3">
-        <v>0.5933503836317136</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>6.615384615384615</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1583,16 +1583,288 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>7.333333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>0.5933503836317136</v>
+      </c>
+      <c r="E9">
+        <v>6.615384615384615</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>0.4066496163682864</v>
+      </c>
+      <c r="E10">
+        <v>6.615384615384615</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>9.384615384615385</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4">
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17">
         <v>0.9415584415584416</v>
       </c>
-      <c r="E4">
+      <c r="E17">
         <v>5.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18">
+        <v>0.05844155844155844</v>
+      </c>
+      <c r="E18">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>